<commit_message>
updates api routes v1/todos
</commit_message>
<xml_diff>
--- a/k8s/MERN-K8s.xlsx
+++ b/k8s/MERN-K8s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrunalmodi/GitHub/mern-app/k8s/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8604B442-C5AC-364C-BE08-7D33967078C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C0A22D-022C-9F4E-84D6-3159325B65DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="4900" windowWidth="28960" windowHeight="15200" xr2:uid="{2ECFAC80-5ECE-2645-9D11-250C06DCBDA0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14380" xr2:uid="{2ECFAC80-5ECE-2645-9D11-250C06DCBDA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DockerHub" sheetId="3" r:id="rId1"/>
@@ -401,32 +401,32 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -749,9 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8680620-5D23-E942-99A4-0758EF20CA80}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -761,189 +759,189 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="18" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="17" t="str">
+      <c r="C5" s="17"/>
+      <c r="D5" s="13" t="str">
         <f>"cd "&amp;B5&amp;"; make build"</f>
         <v>cd frontend; make build</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="18" t="str">
         <f>B5&amp;":latest"</f>
         <v>frontend:latest</v>
       </c>
-      <c r="C6" s="11" t="str">
+      <c r="C6" s="18" t="str">
         <f>"mmodi/"&amp;B5&amp;"-mern-prd:latest"</f>
         <v>mmodi/frontend-mern-prd:latest</v>
       </c>
-      <c r="D6" s="17" t="str">
+      <c r="D6" s="13" t="str">
         <f>"docker tag "&amp;B6&amp;" "&amp;C6</f>
         <v>docker tag frontend:latest mmodi/frontend-mern-prd:latest</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="17" t="str">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="13" t="str">
         <f>"docker push "&amp;C6</f>
         <v>docker push mmodi/frontend-mern-prd:latest</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="17" t="str">
+      <c r="C9" s="17"/>
+      <c r="D9" s="13" t="str">
         <f>"cd "&amp;B9&amp;"; make build"</f>
         <v>cd frontend; make build</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="11" t="str">
+      <c r="B10" s="18" t="str">
         <f>B9&amp;":latest"</f>
         <v>frontend:latest</v>
       </c>
-      <c r="C10" s="11" t="str">
+      <c r="C10" s="18" t="str">
         <f>"mmodi/"&amp;B9&amp;"-mern-dev:latest"</f>
         <v>mmodi/frontend-mern-dev:latest</v>
       </c>
-      <c r="D10" s="17" t="str">
+      <c r="D10" s="13" t="str">
         <f>"docker tag "&amp;B10&amp;" "&amp;C10</f>
         <v>docker tag frontend:latest mmodi/frontend-mern-dev:latest</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="17" t="str">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="13" t="str">
         <f>"docker push "&amp;C10</f>
         <v>docker push mmodi/frontend-mern-dev:latest</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="17" t="str">
+      <c r="C13" s="17"/>
+      <c r="D13" s="13" t="str">
         <f>"cd "&amp;B13&amp;"; make build"</f>
         <v>cd backend; make build</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="11" t="str">
+      <c r="B14" s="18" t="str">
         <f>B13&amp;":latest"</f>
         <v>backend:latest</v>
       </c>
-      <c r="C14" s="11" t="str">
+      <c r="C14" s="18" t="str">
         <f>"mmodi/"&amp;B13&amp;"-mern-prd:latest"</f>
         <v>mmodi/backend-mern-prd:latest</v>
       </c>
-      <c r="D14" s="17" t="str">
+      <c r="D14" s="13" t="str">
         <f>"docker tag "&amp;B14&amp;" "&amp;C14</f>
         <v>docker tag backend:latest mmodi/backend-mern-prd:latest</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="17" t="str">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="13" t="str">
         <f>"docker push "&amp;C14</f>
         <v>docker push mmodi/backend-mern-prd:latest</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{BBB13DA5-54E7-294C-B578-2C747004F954}"/>
@@ -1000,11 +998,11 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -1042,11 +1040,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1096,11 +1094,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1150,11 +1148,11 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -1204,11 +1202,11 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">

</xml_diff>

<commit_message>
prd dev ingress svc
</commit_message>
<xml_diff>
--- a/k8s/MERN-K8s.xlsx
+++ b/k8s/MERN-K8s.xlsx
@@ -8,23 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmodi/GitHub/mern-app/k8s/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4BD685-B369-2D43-9D8D-A4B60C7AC963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C06B954-3A0A-2245-82F5-6DE0B2C0B25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="940" windowWidth="28660" windowHeight="15880" activeTab="1" xr2:uid="{2ECFAC80-5ECE-2645-9D11-250C06DCBDA0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{2ECFAC80-5ECE-2645-9D11-250C06DCBDA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DockerHub-Images" sheetId="5" r:id="rId1"/>
     <sheet name="NetApp-LOD-k8s" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="app_github_repo" localSheetId="1">'NetApp-LOD-k8s'!$C$1</definedName>
-    <definedName name="app_github_repo">#REF!</definedName>
     <definedName name="dr_app_namesace" localSheetId="1">'NetApp-LOD-k8s'!$C$3</definedName>
-    <definedName name="dr_app_namesace">#REF!</definedName>
     <definedName name="external_loadbalancer_namespace" localSheetId="1">'NetApp-LOD-k8s'!$C$4</definedName>
-    <definedName name="external_loadbalancer_namespace">#REF!</definedName>
     <definedName name="prd_app_namesace" localSheetId="1">'NetApp-LOD-k8s'!$C$2</definedName>
-    <definedName name="prd_app_namesace">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,8 +43,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{D560AE0A-78D5-3E4B-8BE5-0480231E6187}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from ClusterIP to LoadBalancer so Metallb can assign an external IP to the NGINX controller.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Step</t>
   </si>
@@ -188,13 +209,37 @@
   </si>
   <si>
     <t>echo "192.168.0.215 prd.myexampleapp.com " &gt;&gt; /etc/hosts</t>
+  </si>
+  <si>
+    <t>PRD-Namespace</t>
+  </si>
+  <si>
+    <t>DEV-Namespace</t>
+  </si>
+  <si>
+    <t>mern-app-prd</t>
+  </si>
+  <si>
+    <t>mern-app-dev</t>
+  </si>
+  <si>
+    <t>Create a namespace for PRD deployments</t>
+  </si>
+  <si>
+    <t>Change the ingress-nginx-controller-admission type</t>
+  </si>
+  <si>
+    <t>Assign DNS using "/etc/hosts"</t>
+  </si>
+  <si>
+    <t>echo "192.168.0.216 dev.myexampleapp.com " &gt;&gt; /etc/hosts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,6 +305,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -879,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4454504A-6B2E-D14F-959F-4BC1D42689EE}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="C1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,6 +940,8 @@
     <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.5" customWidth="1"/>
+    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="124.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1225,4 +1279,252 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F41D8ED-CB82-E640-A77A-F0E814C991DC}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15" t="str">
+        <f>"git clone "&amp;B1</f>
+        <v>git clone https://github.com/mrunal-modi/mern-app</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="15" t="str">
+        <f>"kubectl create ns "&amp;B2</f>
+        <v>kubectl create ns mern-app-prd</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15" t="str">
+        <f>"kubectl apply -f database-pvc.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f database-pvc.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="str">
+        <f>"kubectl apply -f database-deployment.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f database-deployment.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="str">
+        <f>"kubectl apply -f database-service.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f database-service.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="15" t="str">
+        <f>"kubectl apply -f backend-env-configmap.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f backend-env-configmap.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="15" t="str">
+        <f>"kubectl apply -f backend-deployment.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f backend-deployment.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="15" t="str">
+        <f>"kubectl apply -f backend-service.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f backend-service.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="15" t="str">
+        <f>"kubectl apply -f frontend-prd-env-configmap.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f frontend-prd-env-configmap.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="15" t="str">
+        <f>"kubectl apply -f frontend-prd-deployment.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f frontend-prd-deployment.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="15" t="str">
+        <f>"kubectl apply -f frontend-prd-service.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f frontend-prd-service.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="str">
+        <f>"kubectl apply -f ingress.yaml -n "&amp;B2</f>
+        <v>kubectl apply -f ingress.yaml -n mern-app-prd</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="15" t="str">
+        <f>"kubectl apply -f frontend-dev-env-configmap.yaml -n "&amp;B3</f>
+        <v>kubectl apply -f frontend-dev-env-configmap.yaml -n mern-app-dev</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="15" t="str">
+        <f>"kubectl apply -f frontend-dev-deployment.yaml -n "&amp;B3</f>
+        <v>kubectl apply -f frontend-dev-deployment.yaml -n mern-app-dev</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="15" t="str">
+        <f>"kubectl apply -f frontend-dev-service.yaml -n "&amp;B3</f>
+        <v>kubectl apply -f frontend-dev-service.yaml -n mern-app-dev</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="15" t="str">
+        <f>"kubectl apply -f ingress.yaml -n "&amp;B3</f>
+        <v>kubectl apply -f ingress.yaml -n mern-app-dev</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>